<commit_message>
Debris cleaning! VUE recovery
</commit_message>
<xml_diff>
--- a/materials/Информация.xlsx
+++ b/materials/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Команда</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Установить значения HP</t>
-  </si>
-  <si>
-    <t>fakeipl</t>
   </si>
   <si>
     <t>veh</t>
@@ -625,7 +622,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,9 +789,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="18"/>
       <c r="E15" s="25"/>
@@ -802,72 +797,72 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18" s="25"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>34</v>
       </c>
       <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="D20" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>38</v>
       </c>
       <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="D21" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="E21" s="25"/>
     </row>

</xml_diff>

<commit_message>
Command updates and test start
</commit_message>
<xml_diff>
--- a/materials/Информация.xlsx
+++ b/materials/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="254">
   <si>
     <t>Команда</t>
   </si>
@@ -154,6 +154,633 @@
   </si>
   <si>
     <t>Загрузка пропов</t>
+  </si>
+  <si>
+    <t>getbonus</t>
+  </si>
+  <si>
+    <t>lastbonus</t>
+  </si>
+  <si>
+    <t>setbonus</t>
+  </si>
+  <si>
+    <t>createrod</t>
+  </si>
+  <si>
+    <t>sh1</t>
+  </si>
+  <si>
+    <t>vehchange</t>
+  </si>
+  <si>
+    <t>findtrailer</t>
+  </si>
+  <si>
+    <t>bankfix</t>
+  </si>
+  <si>
+    <t>gethwid</t>
+  </si>
+  <si>
+    <t>getsocialclub</t>
+  </si>
+  <si>
+    <t>\---D27</t>
+  </si>
+  <si>
+    <t>loggedinfix</t>
+  </si>
+  <si>
+    <t>vconfigload</t>
+  </si>
+  <si>
+    <t>addpromo</t>
+  </si>
+  <si>
+    <t>giveammo</t>
+  </si>
+  <si>
+    <t>newvnum</t>
+  </si>
+  <si>
+    <t>redname</t>
+  </si>
+  <si>
+    <t>hidenick</t>
+  </si>
+  <si>
+    <t>checkprop</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>setdim</t>
+  </si>
+  <si>
+    <t>checkdim</t>
+  </si>
+  <si>
+    <t>setbizmafia</t>
+  </si>
+  <si>
+    <t>newsimcard</t>
+  </si>
+  <si>
+    <t>takeoffbiz</t>
+  </si>
+  <si>
+    <t>paydaymultiplier</t>
+  </si>
+  <si>
+    <t>expmultiplier</t>
+  </si>
+  <si>
+    <t>offdelfrac</t>
+  </si>
+  <si>
+    <t>removeobj</t>
+  </si>
+  <si>
+    <t>unwarn</t>
+  </si>
+  <si>
+    <t>offunwarn</t>
+  </si>
+  <si>
+    <t>rescar</t>
+  </si>
+  <si>
+    <t>bansync</t>
+  </si>
+  <si>
+    <t>setcolour</t>
+  </si>
+  <si>
+    <t>sc</t>
+  </si>
+  <si>
+    <t>sac</t>
+  </si>
+  <si>
+    <t>checkwanted</t>
+  </si>
+  <si>
+    <t>fixcar</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>admins</t>
+  </si>
+  <si>
+    <t>fixweaponsshops</t>
+  </si>
+  <si>
+    <t>fixgovbizprices</t>
+  </si>
+  <si>
+    <t>deleteproducts</t>
+  </si>
+  <si>
+    <t>changebizprice</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>changestock</t>
+  </si>
+  <si>
+    <t>tpc</t>
+  </si>
+  <si>
+    <t>inv</t>
+  </si>
+  <si>
+    <t>delfrac</t>
+  </si>
+  <si>
+    <t>sendcreator</t>
+  </si>
+  <si>
+    <t>afuel</t>
+  </si>
+  <si>
+    <t>changename</t>
+  </si>
+  <si>
+    <t>startmatwars</t>
+  </si>
+  <si>
+    <t>whitelistdel</t>
+  </si>
+  <si>
+    <t>whitelistadd</t>
+  </si>
+  <si>
+    <t>giveexp</t>
+  </si>
+  <si>
+    <t>housetypeprice</t>
+  </si>
+  <si>
+    <t>delhouseowner</t>
+  </si>
+  <si>
+    <t>svm</t>
+  </si>
+  <si>
+    <t>svn</t>
+  </si>
+  <si>
+    <t>svhid</t>
+  </si>
+  <si>
+    <t>svh</t>
+  </si>
+  <si>
+    <t>delacars</t>
+  </si>
+  <si>
+    <t>delacar</t>
+  </si>
+  <si>
+    <t>delmycars, dmcs</t>
+  </si>
+  <si>
+    <t>allspawncar</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>setfractun</t>
+  </si>
+  <si>
+    <t>newfracveh</t>
+  </si>
+  <si>
+    <t>setfracveh</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>payday</t>
+  </si>
+  <si>
+    <t>giveitem</t>
+  </si>
+  <si>
+    <t>setleader</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>usp</t>
+  </si>
+  <si>
+    <t>metp</t>
+  </si>
+  <si>
+    <t>gethere</t>
+  </si>
+  <si>
+    <t>kill</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>fz</t>
+  </si>
+  <si>
+    <t>ufz</t>
+  </si>
+  <si>
+    <t>setadmin</t>
+  </si>
+  <si>
+    <t>lsn</t>
+  </si>
+  <si>
+    <t>tpcar</t>
+  </si>
+  <si>
+    <t>deladmin</t>
+  </si>
+  <si>
+    <t>setadminrank</t>
+  </si>
+  <si>
+    <t>guns</t>
+  </si>
+  <si>
+    <t>giveclothes</t>
+  </si>
+  <si>
+    <t>setskin</t>
+  </si>
+  <si>
+    <t>oguns</t>
+  </si>
+  <si>
+    <t>delleader</t>
+  </si>
+  <si>
+    <t>deljob</t>
+  </si>
+  <si>
+    <t>vehc</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>mtp2</t>
+  </si>
+  <si>
+    <t>vehhash</t>
+  </si>
+  <si>
+    <t>vehs</t>
+  </si>
+  <si>
+    <t>vehcs</t>
+  </si>
+  <si>
+    <t>vehcustompcolor</t>
+  </si>
+  <si>
+    <t>aclear</t>
+  </si>
+  <si>
+    <t>vehcustomscolor</t>
+  </si>
+  <si>
+    <t>findbyveh</t>
+  </si>
+  <si>
+    <t>vehcustom</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>tp</t>
+  </si>
+  <si>
+    <t>goto</t>
+  </si>
+  <si>
+    <t>flip</t>
+  </si>
+  <si>
+    <t>mtp</t>
+  </si>
+  <si>
+    <t>createunloadpoint</t>
+  </si>
+  <si>
+    <t>createsafe</t>
+  </si>
+  <si>
+    <t>removesafe</t>
+  </si>
+  <si>
+    <t>createstock</t>
+  </si>
+  <si>
+    <t>demorgan</t>
+  </si>
+  <si>
+    <t>loadipl</t>
+  </si>
+  <si>
+    <t>unloadipl</t>
+  </si>
+  <si>
+    <t>loadprop</t>
+  </si>
+  <si>
+    <t>unloadprop</t>
+  </si>
+  <si>
+    <t>starteffect</t>
+  </si>
+  <si>
+    <t>stopeffect</t>
+  </si>
+  <si>
+    <t>udemorgan</t>
+  </si>
+  <si>
+    <t>offjail</t>
+  </si>
+  <si>
+    <t>offwarn</t>
+  </si>
+  <si>
+    <t>ban</t>
+  </si>
+  <si>
+    <t>hardban</t>
+  </si>
+  <si>
+    <t>offban</t>
+  </si>
+  <si>
+    <t>offhardban</t>
+  </si>
+  <si>
+    <t>unban</t>
+  </si>
+  <si>
+    <t>unhardban</t>
+  </si>
+  <si>
+    <t>mute</t>
+  </si>
+  <si>
+    <t>offmute</t>
+  </si>
+  <si>
+    <t>unmute</t>
+  </si>
+  <si>
+    <t>vmute</t>
+  </si>
+  <si>
+    <t>vunmute</t>
+  </si>
+  <si>
+    <t>sban</t>
+  </si>
+  <si>
+    <t>kick</t>
+  </si>
+  <si>
+    <t>skick</t>
+  </si>
+  <si>
+    <t>gm</t>
+  </si>
+  <si>
+    <t>agm</t>
+  </si>
+  <si>
+    <t>warn</t>
+  </si>
+  <si>
+    <t>asms</t>
+  </si>
+  <si>
+    <t>ans</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>setvip</t>
+  </si>
+  <si>
+    <t>checkmoney</t>
+  </si>
+  <si>
+    <t>leave</t>
+  </si>
+  <si>
+    <t>testnotify</t>
+  </si>
+  <si>
+    <t>ticket</t>
+  </si>
+  <si>
+    <t>respawn</t>
+  </si>
+  <si>
+    <t>givemedlic</t>
+  </si>
+  <si>
+    <t>sellbiz</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>ptime</t>
+  </si>
+  <si>
+    <t>sellcars</t>
+  </si>
+  <si>
+    <t>dep</t>
+  </si>
+  <si>
+    <t>gov</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>takegunlic</t>
+  </si>
+  <si>
+    <t>givegunlic</t>
+  </si>
+  <si>
+    <t>pd</t>
+  </si>
+  <si>
+    <t>eject</t>
+  </si>
+  <si>
+    <t>ems</t>
+  </si>
+  <si>
+    <t>pocket</t>
+  </si>
+  <si>
+    <t>buybiz</t>
+  </si>
+  <si>
+    <t>setrank</t>
+  </si>
+  <si>
+    <t>invite</t>
+  </si>
+  <si>
+    <t>uninvite</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>arrest</t>
+  </si>
+  <si>
+    <t>rfp</t>
+  </si>
+  <si>
+    <t>follow</t>
+  </si>
+  <si>
+    <t>unfollow</t>
+  </si>
+  <si>
+    <t>su</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>incar</t>
+  </si>
+  <si>
+    <t>pull</t>
+  </si>
+  <si>
+    <t>warg</t>
+  </si>
+  <si>
+    <t>medkit</t>
+  </si>
+  <si>
+    <t>accept</t>
+  </si>
+  <si>
+    <t>heal</t>
+  </si>
+  <si>
+    <t>capture</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>sellfuel</t>
+  </si>
+  <si>
+    <t>buyfuel</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>cmechanic</t>
+  </si>
+  <si>
+    <t>tprice</t>
+  </si>
+  <si>
+    <t>ta</t>
+  </si>
+  <si>
+    <t>ctaxi</t>
+  </si>
+  <si>
+    <t>taxi</t>
+  </si>
+  <si>
+    <t>orders</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>vh</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>roll</t>
   </si>
 </sst>
 </file>
@@ -234,7 +861,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -270,13 +897,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -348,6 +986,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -631,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,101 +1546,1166 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="18"/>
       <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="18"/>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="18"/>
       <c r="E26" s="25"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C27" s="3"/>
       <c r="D27" s="18"/>
       <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C28" s="3"/>
       <c r="D28" s="18"/>
       <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="18"/>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="18"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
+      <c r="B31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="D31" s="18"/>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C32" s="3"/>
       <c r="D32" s="18"/>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="18"/>
       <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="D34" s="18"/>
       <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C35" s="3"/>
       <c r="D35" s="18"/>
       <c r="E35" s="25"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="C36" s="5"/>
       <c r="D36" s="21"/>
       <c r="E36" s="25"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="21"/>
       <c r="E37" s="25"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="26" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="26" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="26" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="26" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" s="26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" s="26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" s="26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" s="27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174" s="27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B178" s="27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="27" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184" s="27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186" s="27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B188" s="27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190" s="27" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192" s="27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194" s="27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B196" s="27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>253</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Garages code structure updates
</commit_message>
<xml_diff>
--- a/materials/Информация.xlsx
+++ b/materials/Информация.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="257">
   <si>
     <t>Команда</t>
   </si>
@@ -781,6 +781,15 @@
   </si>
   <si>
     <t>roll</t>
+  </si>
+  <si>
+    <t>setgarage</t>
+  </si>
+  <si>
+    <t>creategarage</t>
+  </si>
+  <si>
+    <t>removegarage</t>
   </si>
 </sst>
 </file>
@@ -1275,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E247"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B245" sqref="B245"/>
+      <selection activeCell="B247" sqref="B247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,6 +2716,21 @@
         <v>253</v>
       </c>
     </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>